<commit_message>
new test temperature. hydraulic balance not working
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
+++ b/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D193075-E85F-4EEB-A196-A6EACCBFFA76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED925E3B-F715-4815-BB16-F387DA7D13A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19656" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21528" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8763"/>
   <sheetViews>
-    <sheetView topLeftCell="A582" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A604"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,19 +451,19 @@
         <v>44197</v>
       </c>
       <c r="B4" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C4" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D4" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F4" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3"/>
       <c r="I4" s="3"/>
@@ -474,19 +474,19 @@
         <v>44197.041666666664</v>
       </c>
       <c r="B5" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C5" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D5" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F5" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -36958,8 +36958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5227661-1F4F-4C60-9C9A-A070D4D4BCBF}">
   <dimension ref="A1:F8763"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76:D604"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37020,13 +37020,13 @@
         <v>44197</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -37034,13 +37034,13 @@
         <v>44197.041666666664</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
new data for testing temperature vectors
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
+++ b/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED925E3B-F715-4815-BB16-F387DA7D13A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47E8526-3CFF-4113-B362-EACCD7E6FD4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21528" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23400" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:J8763"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,19 +495,19 @@
         <v>44197.08333321759</v>
       </c>
       <c r="B6" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C6" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D6" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F6" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -516,19 +516,19 @@
         <v>44197.12499971065</v>
       </c>
       <c r="B7" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C7" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D7" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F7" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -536,19 +536,19 @@
         <v>44197.166666261575</v>
       </c>
       <c r="B8" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C8" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D8" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E8" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F8" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -556,19 +556,19 @@
         <v>44197.208332812501</v>
       </c>
       <c r="B9" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C9" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D9" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F9" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -576,19 +576,19 @@
         <v>44197.249999363426</v>
       </c>
       <c r="B10" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C10" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D10" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F10" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -596,19 +596,19 @@
         <v>44197.291665914352</v>
       </c>
       <c r="B11" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C11" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D11" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F11" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -616,19 +616,19 @@
         <v>44197.333332465278</v>
       </c>
       <c r="B12" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C12" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D12" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F12" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -636,19 +636,19 @@
         <v>44197.374999016203</v>
       </c>
       <c r="B13" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C13" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D13" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E13" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F13" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -656,19 +656,19 @@
         <v>44197.416665567129</v>
       </c>
       <c r="B14" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C14" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D14" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F14" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -676,19 +676,19 @@
         <v>44197.458332118054</v>
       </c>
       <c r="B15" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C15" s="3">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="D15" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E15" s="3">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="F15" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
did again some tests
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
+++ b/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ACFF9C-61CF-4779-BD92-FB8AF9E681F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B2A283-347B-4E2B-A8EF-65766ED77078}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30888" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31824" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8763"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E595" sqref="E595"/>
+    <sheetView tabSelected="1" topLeftCell="A478" workbookViewId="0">
+      <selection activeCell="F465" sqref="B465:F479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8802,19 +8802,19 @@
         <v>44213.874933854167</v>
       </c>
       <c r="B409" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C409" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D409" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E409" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F409" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.3">
@@ -8822,19 +8822,19 @@
         <v>44213.91660034722</v>
       </c>
       <c r="B410" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C410" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D410" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E410" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F410" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.3">
@@ -8842,19 +8842,19 @@
         <v>44213.95826684028</v>
       </c>
       <c r="B411" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C411" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D411" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E411" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F411" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.3">
@@ -8862,19 +8862,19 @@
         <v>44213.999933333333</v>
       </c>
       <c r="B412" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C412" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D412" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E412" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F412" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.3">
@@ -8882,19 +8882,19 @@
         <v>44214.041599826392</v>
       </c>
       <c r="B413" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C413" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D413" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E413" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F413" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.3">
@@ -8902,19 +8902,19 @@
         <v>44214.083266319445</v>
       </c>
       <c r="B414" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C414" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D414" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E414" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F414" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.3">
@@ -8922,19 +8922,19 @@
         <v>44214.124932812498</v>
       </c>
       <c r="B415" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C415" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D415" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E415" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F415" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.3">
@@ -8942,19 +8942,19 @@
         <v>44214.166599305558</v>
       </c>
       <c r="B416" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C416" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D416" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E416" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F416" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="417" spans="1:6" x14ac:dyDescent="0.3">
@@ -8962,19 +8962,19 @@
         <v>44214.20826579861</v>
       </c>
       <c r="B417" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C417" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D417" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E417" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F417" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.3">
@@ -8982,19 +8982,19 @@
         <v>44214.24993229167</v>
       </c>
       <c r="B418" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C418" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D418" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E418" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F418" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.3">
@@ -9242,19 +9242,19 @@
         <v>44214.791596701391</v>
       </c>
       <c r="B431" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C431" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D431" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E431" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F431" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.3">
@@ -9262,19 +9262,19 @@
         <v>44214.833263194443</v>
       </c>
       <c r="B432" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C432" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D432" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E432" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F432" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.3">
@@ -9282,19 +9282,19 @@
         <v>44214.874929687503</v>
       </c>
       <c r="B433" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C433" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D433" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E433" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F433" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.3">
@@ -9302,19 +9302,19 @@
         <v>44214.916596180556</v>
       </c>
       <c r="B434" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C434" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D434" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E434" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F434" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.3">
@@ -9322,19 +9322,19 @@
         <v>44214.958262673608</v>
       </c>
       <c r="B435" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C435" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D435" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E435" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F435" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="436" spans="1:6" x14ac:dyDescent="0.3">
@@ -9342,19 +9342,19 @@
         <v>44214.999929166668</v>
       </c>
       <c r="B436" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C436" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D436" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E436" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F436" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="437" spans="1:6" x14ac:dyDescent="0.3">
@@ -9362,19 +9362,19 @@
         <v>44215.041595659721</v>
       </c>
       <c r="B437" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C437" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D437" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E437" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F437" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.3">
@@ -9382,19 +9382,19 @@
         <v>44215.083262152781</v>
       </c>
       <c r="B438" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C438" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D438" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E438" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F438" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="439" spans="1:6" x14ac:dyDescent="0.3">
@@ -9402,19 +9402,19 @@
         <v>44215.124928645833</v>
       </c>
       <c r="B439" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C439" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D439" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E439" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F439" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.3">
@@ -9422,19 +9422,19 @@
         <v>44215.166595138886</v>
       </c>
       <c r="B440" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C440" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D440" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E440" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F440" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="441" spans="1:6" x14ac:dyDescent="0.3">
@@ -9722,19 +9722,19 @@
         <v>44215.791592534719</v>
       </c>
       <c r="B455" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C455" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D455" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E455" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F455" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.3">
@@ -9742,19 +9742,19 @@
         <v>44215.833259027779</v>
       </c>
       <c r="B456" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C456" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D456" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E456" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F456" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.3">
@@ -9762,19 +9762,19 @@
         <v>44215.874925520831</v>
       </c>
       <c r="B457" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C457" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D457" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E457" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F457" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.3">
@@ -9782,19 +9782,19 @@
         <v>44215.916592013891</v>
       </c>
       <c r="B458" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C458" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D458" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E458" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F458" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="459" spans="1:6" x14ac:dyDescent="0.3">
@@ -9802,19 +9802,19 @@
         <v>44215.958258506944</v>
       </c>
       <c r="B459" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C459" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D459" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E459" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F459" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.3">
@@ -9822,19 +9822,19 @@
         <v>44215.999924999996</v>
       </c>
       <c r="B460" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C460" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D460" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E460" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F460" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="461" spans="1:6" x14ac:dyDescent="0.3">
@@ -9842,19 +9842,19 @@
         <v>44216.041591493056</v>
       </c>
       <c r="B461" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C461" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D461" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E461" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F461" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="462" spans="1:6" x14ac:dyDescent="0.3">
@@ -9862,19 +9862,19 @@
         <v>44216.083257986109</v>
       </c>
       <c r="B462" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C462" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D462" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E462" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F462" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="463" spans="1:6" x14ac:dyDescent="0.3">
@@ -9882,19 +9882,19 @@
         <v>44216.124924479169</v>
       </c>
       <c r="B463" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C463" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D463" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E463" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F463" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.3">
@@ -9902,19 +9902,19 @@
         <v>44216.166590972221</v>
       </c>
       <c r="B464" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C464" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D464" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E464" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F464" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.3">
@@ -9922,19 +9922,19 @@
         <v>44216.208257465281</v>
       </c>
       <c r="B465" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C465" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D465" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E465" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F465" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.3">
@@ -9942,19 +9942,19 @@
         <v>44216.249923958334</v>
       </c>
       <c r="B466" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C466" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D466" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E466" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F466" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.3">
@@ -9962,19 +9962,19 @@
         <v>44216.291590451387</v>
       </c>
       <c r="B467" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C467" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D467" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E467" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F467" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.3">
@@ -9982,19 +9982,19 @@
         <v>44216.333256944446</v>
       </c>
       <c r="B468" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C468" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D468" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E468" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F468" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="469" spans="1:6" x14ac:dyDescent="0.3">
@@ -10002,19 +10002,19 @@
         <v>44216.374923437499</v>
       </c>
       <c r="B469" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C469" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D469" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E469" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F469" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="470" spans="1:6" x14ac:dyDescent="0.3">
@@ -10022,19 +10022,19 @@
         <v>44216.416589930559</v>
       </c>
       <c r="B470" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C470" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D470" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E470" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F470" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="471" spans="1:6" x14ac:dyDescent="0.3">
@@ -10042,19 +10042,19 @@
         <v>44216.458256423612</v>
       </c>
       <c r="B471" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C471" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D471" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E471" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F471" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="472" spans="1:6" x14ac:dyDescent="0.3">
@@ -10062,19 +10062,19 @@
         <v>44216.499922916664</v>
       </c>
       <c r="B472" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C472" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D472" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E472" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F472" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="473" spans="1:6" x14ac:dyDescent="0.3">
@@ -10082,19 +10082,19 @@
         <v>44216.541589409724</v>
       </c>
       <c r="B473" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C473" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D473" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E473" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F473" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.3">
@@ -10102,19 +10102,19 @@
         <v>44216.583255902777</v>
       </c>
       <c r="B474" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C474" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D474" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E474" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F474" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="475" spans="1:6" x14ac:dyDescent="0.3">
@@ -10122,19 +10122,19 @@
         <v>44216.624922395837</v>
       </c>
       <c r="B475" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C475" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D475" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E475" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F475" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="476" spans="1:6" x14ac:dyDescent="0.3">
@@ -10142,19 +10142,19 @@
         <v>44216.666588888889</v>
       </c>
       <c r="B476" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C476" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D476" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E476" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F476" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="477" spans="1:6" x14ac:dyDescent="0.3">
@@ -10162,19 +10162,19 @@
         <v>44216.708255381942</v>
       </c>
       <c r="B477" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C477" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D477" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E477" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F477" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="478" spans="1:6" x14ac:dyDescent="0.3">
@@ -10182,19 +10182,19 @@
         <v>44216.749921875002</v>
       </c>
       <c r="B478" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C478" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D478" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E478" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F478" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="479" spans="1:6" x14ac:dyDescent="0.3">
@@ -10202,19 +10202,19 @@
         <v>44216.791588368054</v>
       </c>
       <c r="B479" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C479" s="3">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="D479" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E479" s="3">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F479" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.3">
@@ -10222,19 +10222,19 @@
         <v>44216.833254861114</v>
       </c>
       <c r="B480" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C480" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D480" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E480" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F480" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="481" spans="1:6" x14ac:dyDescent="0.3">
@@ -10242,19 +10242,19 @@
         <v>44216.874921354167</v>
       </c>
       <c r="B481" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C481" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D481" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E481" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F481" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.3">
@@ -10262,19 +10262,19 @@
         <v>44216.916587847219</v>
       </c>
       <c r="B482" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C482" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D482" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E482" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F482" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="483" spans="1:6" x14ac:dyDescent="0.3">
@@ -10282,19 +10282,19 @@
         <v>44216.958254340279</v>
       </c>
       <c r="B483" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C483" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D483" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E483" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F483" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="484" spans="1:6" x14ac:dyDescent="0.3">
@@ -10302,19 +10302,19 @@
         <v>44216.999920833332</v>
       </c>
       <c r="B484" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C484" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D484" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E484" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F484" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="485" spans="1:6" x14ac:dyDescent="0.3">
@@ -10322,19 +10322,19 @@
         <v>44217.041587326392</v>
       </c>
       <c r="B485" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C485" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D485" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E485" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F485" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.3">
@@ -10342,19 +10342,19 @@
         <v>44217.083253819445</v>
       </c>
       <c r="B486" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C486" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D486" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E486" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F486" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="487" spans="1:6" x14ac:dyDescent="0.3">
@@ -10362,19 +10362,19 @@
         <v>44217.124920312497</v>
       </c>
       <c r="B487" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C487" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D487" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E487" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F487" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="488" spans="1:6" x14ac:dyDescent="0.3">
@@ -10382,19 +10382,19 @@
         <v>44217.166586805557</v>
       </c>
       <c r="B488" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C488" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D488" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E488" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F488" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="489" spans="1:6" x14ac:dyDescent="0.3">
@@ -10402,19 +10402,19 @@
         <v>44217.20825329861</v>
       </c>
       <c r="B489" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C489" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D489" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E489" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F489" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="490" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
The test temp updated to test previous commit
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
+++ b/eureca_dhcs/test/input_tests/conditions_temp_test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B2A283-347B-4E2B-A8EF-65766ED77078}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318C009E-DA44-4E45-AA35-8415FC6D1ECF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31824" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38376" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8763"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A478" workbookViewId="0">
-      <selection activeCell="F465" sqref="B465:F479"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:XFD90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1416,13 +1416,13 @@
         <v>44198.999994502316</v>
       </c>
       <c r="B52" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C52" s="3">
         <v>-10</v>
       </c>
       <c r="D52" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E52" s="3">
         <v>-10</v>
@@ -1436,13 +1436,13 @@
         <v>44199.041661053241</v>
       </c>
       <c r="B53" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C53" s="3">
         <v>-10</v>
       </c>
       <c r="D53" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E53" s="3">
         <v>-10</v>
@@ -1456,13 +1456,13 @@
         <v>44199.083327604167</v>
       </c>
       <c r="B54" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C54" s="3">
         <v>-10</v>
       </c>
       <c r="D54" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E54" s="3">
         <v>-10</v>
@@ -1476,13 +1476,13 @@
         <v>44199.124994155092</v>
       </c>
       <c r="B55" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C55" s="3">
         <v>-10</v>
       </c>
       <c r="D55" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E55" s="3">
         <v>-10</v>
@@ -1496,13 +1496,13 @@
         <v>44199.166660706018</v>
       </c>
       <c r="B56" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C56" s="3">
         <v>-10</v>
       </c>
       <c r="D56" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E56" s="3">
         <v>-10</v>
@@ -1516,13 +1516,13 @@
         <v>44199.208327256943</v>
       </c>
       <c r="B57" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C57" s="3">
         <v>-10</v>
       </c>
       <c r="D57" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E57" s="3">
         <v>-10</v>
@@ -1536,13 +1536,13 @@
         <v>44199.249993807869</v>
       </c>
       <c r="B58" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C58" s="3">
         <v>-10</v>
       </c>
       <c r="D58" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E58" s="3">
         <v>-10</v>
@@ -1556,13 +1556,13 @@
         <v>44199.291660358795</v>
       </c>
       <c r="B59" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C59" s="3">
         <v>-10</v>
       </c>
       <c r="D59" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E59" s="3">
         <v>-10</v>
@@ -1576,13 +1576,13 @@
         <v>44199.33332690972</v>
       </c>
       <c r="B60" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C60" s="3">
         <v>-10</v>
       </c>
       <c r="D60" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E60" s="3">
         <v>-10</v>
@@ -1596,13 +1596,13 @@
         <v>44199.374993460646</v>
       </c>
       <c r="B61" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C61" s="3">
         <v>-10</v>
       </c>
       <c r="D61" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E61" s="3">
         <v>-10</v>
@@ -1616,13 +1616,13 @@
         <v>44199.416660011571</v>
       </c>
       <c r="B62" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C62" s="3">
         <v>-10</v>
       </c>
       <c r="D62" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E62" s="3">
         <v>-10</v>
@@ -1636,13 +1636,13 @@
         <v>44199.458326562497</v>
       </c>
       <c r="B63" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C63" s="3">
         <v>-10</v>
       </c>
       <c r="D63" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E63" s="3">
         <v>-10</v>
@@ -1656,13 +1656,13 @@
         <v>44199.499993113423</v>
       </c>
       <c r="B64" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C64" s="3">
         <v>-10</v>
       </c>
       <c r="D64" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E64" s="3">
         <v>-10</v>
@@ -1676,13 +1676,13 @@
         <v>44199.541659664355</v>
       </c>
       <c r="B65" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C65" s="3">
         <v>-10</v>
       </c>
       <c r="D65" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E65" s="3">
         <v>-10</v>
@@ -1696,13 +1696,13 @@
         <v>44199.583326215281</v>
       </c>
       <c r="B66" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C66" s="3">
         <v>-10</v>
       </c>
       <c r="D66" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E66" s="3">
         <v>-10</v>
@@ -1716,13 +1716,13 @@
         <v>44199.624992766207</v>
       </c>
       <c r="B67" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C67" s="3">
         <v>-10</v>
       </c>
       <c r="D67" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E67" s="3">
         <v>-10</v>
@@ -1736,13 +1736,13 @@
         <v>44199.666659317132</v>
       </c>
       <c r="B68" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C68" s="3">
         <v>-10</v>
       </c>
       <c r="D68" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E68" s="3">
         <v>-10</v>
@@ -1756,13 +1756,13 @@
         <v>44199.708325868058</v>
       </c>
       <c r="B69" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C69" s="3">
         <v>-10</v>
       </c>
       <c r="D69" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E69" s="3">
         <v>-10</v>
@@ -1776,13 +1776,13 @@
         <v>44199.749992418983</v>
       </c>
       <c r="B70" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C70" s="3">
         <v>-10</v>
       </c>
       <c r="D70" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E70" s="3">
         <v>-10</v>
@@ -37204,8 +37204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5227661-1F4F-4C60-9C9A-A070D4D4BCBF}">
   <dimension ref="A1:F8763"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90:B604"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37294,7 +37294,7 @@
         <v>44197.08333321759</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -37308,7 +37308,7 @@
         <v>44197.12499971065</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -37322,7 +37322,7 @@
         <v>44197.166666261575</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -37336,7 +37336,7 @@
         <v>44197.208332812501</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -37350,7 +37350,7 @@
         <v>44197.249999363426</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -37364,7 +37364,7 @@
         <v>44197.291665914352</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11">
         <v>50</v>
@@ -37378,7 +37378,7 @@
         <v>44197.333332465278</v>
       </c>
       <c r="B12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -37392,7 +37392,7 @@
         <v>44197.374999016203</v>
       </c>
       <c r="B13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13">
         <v>50</v>
@@ -37406,7 +37406,7 @@
         <v>44197.416665567129</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>50</v>
@@ -37420,7 +37420,7 @@
         <v>44197.458332118054</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>50</v>
@@ -37434,7 +37434,7 @@
         <v>44197.49999866898</v>
       </c>
       <c r="B16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16">
         <v>50</v>
@@ -37448,7 +37448,7 @@
         <v>44197.541665219906</v>
       </c>
       <c r="B17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17">
         <v>50</v>
@@ -37462,7 +37462,7 @@
         <v>44197.583331770831</v>
       </c>
       <c r="B18">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>50</v>
@@ -37476,7 +37476,7 @@
         <v>44197.624998321757</v>
       </c>
       <c r="B19">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19">
         <v>50</v>
@@ -37490,7 +37490,7 @@
         <v>44197.666664872682</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>50</v>
@@ -37504,7 +37504,7 @@
         <v>44197.708331423608</v>
       </c>
       <c r="B21">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>50</v>
@@ -37518,7 +37518,7 @@
         <v>44197.749997974533</v>
       </c>
       <c r="B22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22">
         <v>50</v>
@@ -37532,7 +37532,7 @@
         <v>44197.791664525466</v>
       </c>
       <c r="B23">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23">
         <v>50</v>
@@ -37546,7 +37546,7 @@
         <v>44197.833331076392</v>
       </c>
       <c r="B24">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24">
         <v>50</v>
@@ -37560,7 +37560,7 @@
         <v>44197.874997627317</v>
       </c>
       <c r="B25">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25">
         <v>50</v>
@@ -37574,7 +37574,7 @@
         <v>44197.916664178243</v>
       </c>
       <c r="B26">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C26">
         <v>50</v>
@@ -37588,7 +37588,7 @@
         <v>44197.958330729169</v>
       </c>
       <c r="B27">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>50</v>
@@ -37602,7 +37602,7 @@
         <v>44197.999997280094</v>
       </c>
       <c r="B28">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28">
         <v>50</v>
@@ -37616,7 +37616,7 @@
         <v>44198.04166383102</v>
       </c>
       <c r="B29">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C29">
         <v>50</v>
@@ -37630,7 +37630,7 @@
         <v>44198.083330381945</v>
       </c>
       <c r="B30">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <v>50</v>
@@ -37644,7 +37644,7 @@
         <v>44198.124996932871</v>
       </c>
       <c r="B31">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31">
         <v>50</v>
@@ -37658,7 +37658,7 @@
         <v>44198.166663483797</v>
       </c>
       <c r="B32">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C32">
         <v>50</v>
@@ -37672,7 +37672,7 @@
         <v>44198.208330034722</v>
       </c>
       <c r="B33">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <v>50</v>
@@ -37686,7 +37686,7 @@
         <v>44198.249996585648</v>
       </c>
       <c r="B34">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C34">
         <v>50</v>
@@ -37700,7 +37700,7 @@
         <v>44198.291663136573</v>
       </c>
       <c r="B35">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C35">
         <v>50</v>
@@ -37714,7 +37714,7 @@
         <v>44198.333329687499</v>
       </c>
       <c r="B36">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C36">
         <v>50</v>
@@ -37728,7 +37728,7 @@
         <v>44198.374996238425</v>
       </c>
       <c r="B37">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C37">
         <v>50</v>
@@ -37742,7 +37742,7 @@
         <v>44198.41666278935</v>
       </c>
       <c r="B38">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C38">
         <v>50</v>
@@ -37756,7 +37756,7 @@
         <v>44198.458329340276</v>
       </c>
       <c r="B39">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>50</v>
@@ -37770,7 +37770,7 @@
         <v>44198.499995891201</v>
       </c>
       <c r="B40">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C40">
         <v>50</v>
@@ -37784,7 +37784,7 @@
         <v>44198.541662442127</v>
       </c>
       <c r="B41">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -37798,7 +37798,7 @@
         <v>44198.583328993052</v>
       </c>
       <c r="B42">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C42">
         <v>50</v>
@@ -37812,7 +37812,7 @@
         <v>44198.624995543978</v>
       </c>
       <c r="B43">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C43">
         <v>50</v>
@@ -37826,7 +37826,7 @@
         <v>44198.666662094911</v>
       </c>
       <c r="B44">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C44">
         <v>50</v>
@@ -37840,7 +37840,7 @@
         <v>44198.708328645836</v>
       </c>
       <c r="B45">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C45">
         <v>50</v>
@@ -37854,7 +37854,7 @@
         <v>44198.749995196762</v>
       </c>
       <c r="B46">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C46">
         <v>50</v>
@@ -37868,7 +37868,7 @@
         <v>44198.791661747688</v>
       </c>
       <c r="B47">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C47">
         <v>50</v>
@@ -37882,7 +37882,7 @@
         <v>44198.833328298613</v>
       </c>
       <c r="B48">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C48">
         <v>50</v>
@@ -37896,7 +37896,7 @@
         <v>44198.874994849539</v>
       </c>
       <c r="B49">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>50</v>
@@ -37910,7 +37910,7 @@
         <v>44198.916661400464</v>
       </c>
       <c r="B50">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C50">
         <v>50</v>
@@ -37924,7 +37924,7 @@
         <v>44198.95832795139</v>
       </c>
       <c r="B51">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -37938,7 +37938,7 @@
         <v>44198.999994502316</v>
       </c>
       <c r="B52">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C52">
         <v>50</v>
@@ -37952,7 +37952,7 @@
         <v>44199.041661053241</v>
       </c>
       <c r="B53">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C53">
         <v>50</v>
@@ -37966,7 +37966,7 @@
         <v>44199.083327604167</v>
       </c>
       <c r="B54">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C54">
         <v>50</v>
@@ -37980,7 +37980,7 @@
         <v>44199.124994155092</v>
       </c>
       <c r="B55">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C55">
         <v>50</v>
@@ -37994,7 +37994,7 @@
         <v>44199.166660706018</v>
       </c>
       <c r="B56">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C56">
         <v>50</v>
@@ -38008,7 +38008,7 @@
         <v>44199.208327256943</v>
       </c>
       <c r="B57">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C57">
         <v>50</v>
@@ -38022,7 +38022,7 @@
         <v>44199.249993807869</v>
       </c>
       <c r="B58">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C58">
         <v>50</v>
@@ -38036,7 +38036,7 @@
         <v>44199.291660358795</v>
       </c>
       <c r="B59">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C59">
         <v>50</v>
@@ -38050,7 +38050,7 @@
         <v>44199.33332690972</v>
       </c>
       <c r="B60">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C60">
         <v>50</v>
@@ -38064,7 +38064,7 @@
         <v>44199.374993460646</v>
       </c>
       <c r="B61">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C61">
         <v>50</v>
@@ -38078,7 +38078,7 @@
         <v>44199.416660011571</v>
       </c>
       <c r="B62">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C62">
         <v>50</v>
@@ -38092,7 +38092,7 @@
         <v>44199.458326562497</v>
       </c>
       <c r="B63">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C63">
         <v>50</v>
@@ -38106,7 +38106,7 @@
         <v>44199.499993113423</v>
       </c>
       <c r="B64">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C64">
         <v>50</v>
@@ -38120,7 +38120,7 @@
         <v>44199.541659664355</v>
       </c>
       <c r="B65">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C65">
         <v>50</v>
@@ -38134,7 +38134,7 @@
         <v>44199.583326215281</v>
       </c>
       <c r="B66">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C66">
         <v>50</v>
@@ -38148,7 +38148,7 @@
         <v>44199.624992766207</v>
       </c>
       <c r="B67">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C67">
         <v>50</v>
@@ -38162,7 +38162,7 @@
         <v>44199.666659317132</v>
       </c>
       <c r="B68">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C68">
         <v>50</v>
@@ -38176,7 +38176,7 @@
         <v>44199.708325868058</v>
       </c>
       <c r="B69">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C69">
         <v>50</v>
@@ -38190,7 +38190,7 @@
         <v>44199.749992418983</v>
       </c>
       <c r="B70">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C70">
         <v>50</v>
@@ -38204,7 +38204,7 @@
         <v>44199.791658969909</v>
       </c>
       <c r="B71">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C71">
         <v>50</v>
@@ -38218,7 +38218,7 @@
         <v>44199.833325520834</v>
       </c>
       <c r="B72">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C72">
         <v>50</v>
@@ -38232,7 +38232,7 @@
         <v>44199.87499207176</v>
       </c>
       <c r="B73">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C73">
         <v>50</v>
@@ -38246,7 +38246,7 @@
         <v>44199.916658622686</v>
       </c>
       <c r="B74">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C74">
         <v>50</v>
@@ -38260,7 +38260,7 @@
         <v>44199.958325173611</v>
       </c>
       <c r="B75">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C75">
         <v>50</v>
@@ -38274,7 +38274,7 @@
         <v>44199.999991724537</v>
       </c>
       <c r="B76">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C76">
         <v>50</v>
@@ -38288,7 +38288,7 @@
         <v>44200.041658159724</v>
       </c>
       <c r="B77">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C77">
         <v>50</v>
@@ -38302,7 +38302,7 @@
         <v>44200.083324652776</v>
       </c>
       <c r="B78">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C78">
         <v>50</v>
@@ -38316,7 +38316,7 @@
         <v>44200.124991145836</v>
       </c>
       <c r="B79">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C79">
         <v>50</v>
@@ -38330,7 +38330,7 @@
         <v>44200.166657638889</v>
       </c>
       <c r="B80">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C80">
         <v>50</v>
@@ -38344,7 +38344,7 @@
         <v>44200.208324131941</v>
       </c>
       <c r="B81">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C81">
         <v>50</v>
@@ -38358,7 +38358,7 @@
         <v>44200.249990625001</v>
       </c>
       <c r="B82">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C82">
         <v>50</v>
@@ -38372,7 +38372,7 @@
         <v>44200.291657118054</v>
       </c>
       <c r="B83">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C83">
         <v>50</v>
@@ -38386,7 +38386,7 @@
         <v>44200.333323611114</v>
       </c>
       <c r="B84">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C84">
         <v>50</v>
@@ -38400,7 +38400,7 @@
         <v>44200.374990104166</v>
       </c>
       <c r="B85">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C85">
         <v>50</v>
@@ -38414,7 +38414,7 @@
         <v>44200.416656597219</v>
       </c>
       <c r="B86">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C86">
         <v>50</v>
@@ -38428,7 +38428,7 @@
         <v>44200.458323090279</v>
       </c>
       <c r="B87">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C87">
         <v>50</v>
@@ -38442,7 +38442,7 @@
         <v>44200.499989583332</v>
       </c>
       <c r="B88">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C88">
         <v>50</v>
@@ -38456,7 +38456,7 @@
         <v>44200.541656076392</v>
       </c>
       <c r="B89">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C89">
         <v>50</v>

</xml_diff>